<commit_message>
maj template comment à la fin
</commit_message>
<xml_diff>
--- a/template_pegase_v1/bloodgases.xlsx
+++ b/template_pegase_v1/bloodgases.xlsx
@@ -41,18 +41,18 @@
     <t>SampleID</t>
   </si>
   <si>
+    <t>WaitingTime</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>WaitingTime</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t># Date de l'analyse</t>
   </si>
   <si>
@@ -80,10 +80,10 @@
     <t># Identifiant de l'echantillon</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t># Commentaire</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>#date</t>
@@ -280,10 +280,10 @@
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
@@ -318,16 +318,16 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -359,16 +359,16 @@
         <v>37</v>
       </c>
       <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
         <v>38</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -400,16 +400,16 @@
         <v>47</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>